<commit_message>
Adding fixed data for season 2016-2017
</commit_message>
<xml_diff>
--- a/lf_front/data/fixed/2016-2017/Spelerslijst basisopstellingen.xlsx
+++ b/lf_front/data/fixed/2016-2017/Spelerslijst basisopstellingen.xlsx
@@ -9,6 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="ontbrekende" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="206">
   <si>
     <t>player_playerId</t>
   </si>
@@ -548,6 +549,96 @@
   </si>
   <si>
     <t>Wit-Wit 3G</t>
+  </si>
+  <si>
+    <t>4GHENT 4G</t>
+  </si>
+  <si>
+    <t>Geraardsbergen 1G</t>
+  </si>
+  <si>
+    <t>Geraardsbergen 1H</t>
+  </si>
+  <si>
+    <t>Geraardsbergen 2H</t>
+  </si>
+  <si>
+    <t>Lede 1G</t>
+  </si>
+  <si>
+    <t>Lede 1H</t>
+  </si>
+  <si>
+    <t>Oudegem 1D</t>
+  </si>
+  <si>
+    <t>Oudegem 2D</t>
+  </si>
+  <si>
+    <t>Oudegem 2G</t>
+  </si>
+  <si>
+    <t>Oudegem 2H</t>
+  </si>
+  <si>
+    <t>Oudegem 3G</t>
+  </si>
+  <si>
+    <t>Oudegem 3H</t>
+  </si>
+  <si>
+    <t>Oudegem 4G</t>
+  </si>
+  <si>
+    <t>Oudegem 4H</t>
+  </si>
+  <si>
+    <t>Oudegem 5G</t>
+  </si>
+  <si>
+    <t>Pluimplukkers 3D</t>
+  </si>
+  <si>
+    <t>Pluimplukkers 4D</t>
+  </si>
+  <si>
+    <t>Pluimplukkers 4G</t>
+  </si>
+  <si>
+    <t>Pluimplukkers 4H</t>
+  </si>
+  <si>
+    <t>Pluimplukkers 5G</t>
+  </si>
+  <si>
+    <t>Pluimplukkers 5H</t>
+  </si>
+  <si>
+    <t>Pluimplukkers 6G</t>
+  </si>
+  <si>
+    <t>Pluimplukkers 6H</t>
+  </si>
+  <si>
+    <t>Pluimplukkers 7G</t>
+  </si>
+  <si>
+    <t>Pluimplukkers 7H</t>
+  </si>
+  <si>
+    <t>Pluimplukkers 8G</t>
+  </si>
+  <si>
+    <t>Pluimplukkers 9G</t>
+  </si>
+  <si>
+    <t>Smash For Fun 1D</t>
+  </si>
+  <si>
+    <t>Smash For Fun 1G</t>
+  </si>
+  <si>
+    <t>Smash For Fun 1H</t>
   </si>
 </sst>
 </file>
@@ -815,14 +906,14 @@
   </sheetPr>
   <dimension ref="A1:E693"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A483" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G519" activeCellId="0" sqref="G519"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.417004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="27.6356275303644"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="27.8502024291498"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="2" width="8.89068825910931"/>
   </cols>
   <sheetData>
@@ -7821,4 +7912,182 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A30"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.8825910931174"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.1417004048583"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="3" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="3" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="3" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="3" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="3" t="s">
+        <v>205</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding fixed data for season 2016-2017, adding Wallabies 1G, corrections Wetteren 2G en 3G, liga team 4GHENT 1D
</commit_message>
<xml_diff>
--- a/lf_front/data/fixed/2016-2017/Spelerslijst basisopstellingen.xlsx
+++ b/lf_front/data/fixed/2016-2017/Spelerslijst basisopstellingen.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="209">
   <si>
     <t>player_playerId</t>
   </si>
@@ -649,13 +649,16 @@
   </si>
   <si>
     <t>Smash For Fun 2G</t>
+  </si>
+  <si>
+    <t>Wallabies 1G</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -687,6 +690,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF505050"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -732,7 +741,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -766,6 +775,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -1149,10 +1159,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK825"/>
+  <dimension ref="A1:AMK829"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A267" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A735" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B752" sqref="B752"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8721,664 +8731,706 @@
       <c r="E757"/>
     </row>
     <row r="758" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A758" s="15">
-        <v>50039675</v>
+      <c r="A758" s="5">
+        <v>50109956</v>
       </c>
       <c r="B758" s="2" t="s">
-        <v>158</v>
+        <v>208</v>
       </c>
       <c r="D758"/>
       <c r="E758"/>
     </row>
     <row r="759" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A759" s="15">
-        <v>50109183</v>
+      <c r="A759" s="5">
+        <v>50043699</v>
       </c>
       <c r="B759" s="2" t="s">
-        <v>158</v>
+        <v>208</v>
       </c>
       <c r="D759"/>
       <c r="E759"/>
     </row>
     <row r="760" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A760" s="15">
-        <v>50107383</v>
+      <c r="A760" s="5">
+        <v>50109169</v>
       </c>
       <c r="B760" s="2" t="s">
-        <v>158</v>
+        <v>208</v>
       </c>
       <c r="D760"/>
       <c r="E760"/>
     </row>
     <row r="761" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A761" s="15">
-        <v>50025471</v>
+      <c r="A761" s="5">
+        <v>50045008</v>
       </c>
       <c r="B761" s="2" t="s">
-        <v>158</v>
+        <v>208</v>
       </c>
       <c r="D761"/>
       <c r="E761"/>
     </row>
     <row r="762" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A762" s="15">
-        <v>50106208</v>
+      <c r="A762" s="5">
+        <v>50039675</v>
       </c>
       <c r="B762" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D762"/>
       <c r="E762"/>
     </row>
     <row r="763" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A763" s="15">
-        <v>50022624</v>
+      <c r="A763" s="5">
+        <v>50109183</v>
       </c>
       <c r="B763" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D763"/>
       <c r="E763"/>
     </row>
     <row r="764" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A764" s="15">
-        <v>50094130</v>
+      <c r="A764" s="5">
+        <v>50107383</v>
       </c>
       <c r="B764" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D764"/>
       <c r="E764"/>
     </row>
     <row r="765" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A765" s="15">
-        <v>50087097</v>
+        <v>50025471</v>
       </c>
       <c r="B765" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D765"/>
       <c r="E765"/>
     </row>
     <row r="766" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A766" s="15">
-        <v>50053285</v>
+        <v>50106208</v>
       </c>
       <c r="B766" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D766"/>
       <c r="E766"/>
     </row>
     <row r="767" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A767" s="15">
-        <v>50075482</v>
+        <v>50022624</v>
       </c>
       <c r="B767" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D767"/>
       <c r="E767"/>
     </row>
     <row r="768" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A768" s="15">
-        <v>50048239</v>
+        <v>50094130</v>
       </c>
       <c r="B768" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D768"/>
       <c r="E768"/>
     </row>
     <row r="769" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A769" s="15">
-        <v>50064536</v>
+        <v>50087097</v>
       </c>
       <c r="B769" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D769"/>
       <c r="E769"/>
     </row>
     <row r="770" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A770" s="15">
-        <v>50089584</v>
+        <v>50053285</v>
       </c>
       <c r="B770" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D770"/>
       <c r="E770"/>
     </row>
     <row r="771" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A771" s="15">
-        <v>50053284</v>
+        <v>50075482</v>
       </c>
       <c r="B771" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D771"/>
       <c r="E771"/>
     </row>
     <row r="772" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A772" s="15">
-        <v>50075199</v>
+        <v>50048239</v>
       </c>
       <c r="B772" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D772"/>
       <c r="E772"/>
     </row>
     <row r="773" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A773" s="15">
-        <v>50076756</v>
+        <v>50064536</v>
       </c>
       <c r="B773" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D773"/>
       <c r="E773"/>
     </row>
     <row r="774" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A774" s="15">
-        <v>50072795</v>
+        <v>50089584</v>
       </c>
       <c r="B774" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D774"/>
       <c r="E774"/>
     </row>
     <row r="775" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A775" s="15">
-        <v>50054430</v>
+        <v>50053284</v>
       </c>
       <c r="B775" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D775"/>
       <c r="E775"/>
     </row>
     <row r="776" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A776" s="15">
-        <v>50048231</v>
+        <v>50075199</v>
       </c>
       <c r="B776" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D776"/>
       <c r="E776"/>
     </row>
     <row r="777" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A777" s="15">
-        <v>50032887</v>
+        <v>50076756</v>
       </c>
       <c r="B777" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D777"/>
       <c r="E777"/>
     </row>
     <row r="778" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A778" s="15">
-        <v>50106193</v>
+        <v>50072795</v>
       </c>
       <c r="B778" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D778"/>
       <c r="E778"/>
     </row>
     <row r="779" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A779" s="15">
-        <v>50087085</v>
+        <v>50054430</v>
       </c>
       <c r="B779" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D779"/>
       <c r="E779"/>
     </row>
     <row r="780" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A780" s="11">
-        <v>50356798</v>
+      <c r="A780" s="15">
+        <v>50048231</v>
       </c>
       <c r="B780" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D780"/>
       <c r="E780"/>
     </row>
     <row r="781" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A781" s="11">
-        <v>50454803</v>
+      <c r="A781" s="15">
+        <v>50032887</v>
       </c>
       <c r="B781" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D781"/>
       <c r="E781"/>
     </row>
     <row r="782" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A782" s="15">
-        <v>50061714</v>
+        <v>50106193</v>
       </c>
       <c r="B782" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D782"/>
       <c r="E782"/>
     </row>
     <row r="783" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A783" s="15">
-        <v>50095147</v>
+        <v>50087085</v>
       </c>
       <c r="B783" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D783"/>
       <c r="E783"/>
     </row>
     <row r="784" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A784" s="15">
-        <v>50053943</v>
+      <c r="A784" s="11">
+        <v>50356798</v>
       </c>
       <c r="B784" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D784"/>
       <c r="E784"/>
     </row>
     <row r="785" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A785" s="15">
-        <v>50094761</v>
+      <c r="A785" s="11">
+        <v>50454803</v>
       </c>
       <c r="B785" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D785"/>
       <c r="E785"/>
     </row>
     <row r="786" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A786" s="15">
-        <v>50110722</v>
+        <v>50061714</v>
       </c>
       <c r="B786" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D786"/>
       <c r="E786"/>
     </row>
     <row r="787" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A787" s="15">
-        <v>50251708</v>
+        <v>50095147</v>
       </c>
       <c r="B787" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D787"/>
       <c r="E787"/>
     </row>
     <row r="788" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A788" s="15">
-        <v>50057897</v>
+        <v>50053943</v>
       </c>
       <c r="B788" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D788"/>
       <c r="E788"/>
     </row>
     <row r="789" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A789" s="15">
-        <v>50032878</v>
+        <v>50094761</v>
       </c>
       <c r="B789" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D789"/>
       <c r="E789"/>
     </row>
     <row r="790" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A790" s="15">
-        <v>50102325</v>
+        <v>50110722</v>
       </c>
       <c r="B790" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D790"/>
       <c r="E790"/>
     </row>
     <row r="791" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A791" s="15">
-        <v>50072192</v>
+        <v>50251708</v>
       </c>
       <c r="B791" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D791"/>
       <c r="E791"/>
     </row>
     <row r="792" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A792" s="15">
-        <v>50092902</v>
+        <v>50057897</v>
       </c>
       <c r="B792" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D792"/>
       <c r="E792"/>
     </row>
     <row r="793" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A793" s="15">
-        <v>50529374</v>
+        <v>50032878</v>
       </c>
       <c r="B793" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D793"/>
       <c r="E793"/>
     </row>
     <row r="794" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A794" s="15">
-        <v>50039675</v>
+        <v>50102325</v>
       </c>
       <c r="B794" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D794"/>
       <c r="E794"/>
     </row>
     <row r="795" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A795" s="15">
-        <v>50109183</v>
+        <v>50072192</v>
       </c>
       <c r="B795" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D795"/>
       <c r="E795"/>
     </row>
     <row r="796" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A796" s="15">
-        <v>50053943</v>
+        <v>50092902</v>
       </c>
       <c r="B796" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D796"/>
       <c r="E796"/>
     </row>
     <row r="797" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A797" s="15">
-        <v>50061714</v>
+        <v>50529374</v>
       </c>
       <c r="B797" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D797"/>
       <c r="E797"/>
     </row>
     <row r="798" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A798" s="15">
-        <v>50022624</v>
+        <v>50039675</v>
       </c>
       <c r="B798" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D798"/>
       <c r="E798"/>
     </row>
     <row r="799" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A799" s="15">
-        <v>50107383</v>
+        <v>50109183</v>
       </c>
       <c r="B799" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D799"/>
       <c r="E799"/>
     </row>
     <row r="800" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A800" s="15">
-        <v>50110722</v>
+        <v>50053943</v>
       </c>
       <c r="B800" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D800"/>
       <c r="E800"/>
     </row>
     <row r="801" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A801" s="15">
-        <v>50094761</v>
+        <v>50061714</v>
       </c>
       <c r="B801" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D801"/>
       <c r="E801"/>
     </row>
     <row r="802" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A802" s="15">
-        <v>50106208</v>
+        <v>50022624</v>
       </c>
       <c r="B802" s="2" t="s">
-        <v>169</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="C802" s="19"/>
       <c r="D802"/>
       <c r="E802"/>
     </row>
     <row r="803" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A803" s="15">
-        <v>50053285</v>
+        <v>50106208</v>
       </c>
       <c r="B803" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D803"/>
       <c r="E803"/>
     </row>
     <row r="804" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A804" s="15">
-        <v>50251708</v>
+        <v>50110722</v>
       </c>
       <c r="B804" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D804"/>
       <c r="E804"/>
     </row>
     <row r="805" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A805" s="15">
-        <v>50095147</v>
+        <v>50094761</v>
       </c>
       <c r="B805" s="2" t="s">
-        <v>169</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="C805" s="19"/>
       <c r="D805"/>
       <c r="E805"/>
     </row>
     <row r="806" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A806" s="11">
-        <v>50102832</v>
-      </c>
-      <c r="B806" s="7" t="s">
-        <v>170</v>
+      <c r="A806" s="15">
+        <v>50107383</v>
+      </c>
+      <c r="B806" s="2" t="s">
+        <v>169</v>
       </c>
       <c r="D806"/>
       <c r="E806"/>
     </row>
     <row r="807" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A807" s="13">
-        <v>50093915</v>
+      <c r="A807" s="15">
+        <v>50053285</v>
       </c>
       <c r="B807" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D807"/>
       <c r="E807"/>
     </row>
     <row r="808" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A808" s="13">
-        <v>50075806</v>
+      <c r="A808" s="15">
+        <v>50251708</v>
       </c>
       <c r="B808" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D808"/>
       <c r="E808"/>
     </row>
     <row r="809" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A809" s="11">
-        <v>50057037</v>
+      <c r="A809" s="15">
+        <v>50095147</v>
       </c>
       <c r="B809" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D809"/>
       <c r="E809"/>
     </row>
     <row r="810" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A810" s="11">
-        <v>50060380</v>
-      </c>
-      <c r="B810" s="2" t="s">
-        <v>171</v>
+        <v>50102832</v>
+      </c>
+      <c r="B810" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="D810"/>
       <c r="E810"/>
     </row>
     <row r="811" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A811" s="13">
-        <v>50094834</v>
+        <v>50093915</v>
       </c>
       <c r="B811" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D811"/>
       <c r="E811"/>
     </row>
     <row r="812" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A812" s="11">
-        <v>50058094</v>
+      <c r="A812" s="15">
+        <v>50075806</v>
       </c>
       <c r="B812" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D812"/>
       <c r="E812"/>
     </row>
     <row r="813" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A813" s="11">
-        <v>50039511</v>
+        <v>50057037</v>
       </c>
       <c r="B813" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="D813" s="16"/>
-      <c r="E813" s="17"/>
+        <v>170</v>
+      </c>
+      <c r="D813"/>
+      <c r="E813"/>
     </row>
     <row r="814" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A814" s="11">
-        <v>50029666</v>
+        <v>50060380</v>
       </c>
       <c r="B814" s="2" t="s">
-        <v>172</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="D814"/>
+      <c r="E814"/>
     </row>
     <row r="815" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A815" s="13">
+        <v>50094834</v>
+      </c>
+      <c r="B815" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D815"/>
+      <c r="E815"/>
+    </row>
+    <row r="816" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A816" s="11">
+        <v>50058094</v>
+      </c>
+      <c r="B816" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D816"/>
+      <c r="E816"/>
+    </row>
+    <row r="817" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A817" s="11">
+        <v>50039511</v>
+      </c>
+      <c r="B817" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D817" s="16"/>
+      <c r="E817" s="17"/>
+    </row>
+    <row r="818" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A818" s="11">
+        <v>50029666</v>
+      </c>
+      <c r="B818" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="819" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A819" s="13">
         <v>50106212</v>
       </c>
-      <c r="B815" s="2" t="s">
+      <c r="B819" s="2" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="816" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A816" s="13">
+    <row r="820" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A820" s="13">
         <v>50114875</v>
       </c>
-      <c r="B816" s="2" t="s">
+      <c r="B820" s="2" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="817" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A817" s="11">
+    <row r="821" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A821" s="11">
         <v>50091937</v>
       </c>
-      <c r="B817" s="2" t="s">
+      <c r="B821" s="2" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="818" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A818" s="11">
+    <row r="822" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A822" s="11">
         <v>50055223</v>
       </c>
-      <c r="B818" s="2" t="s">
+      <c r="B822" s="2" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="819" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A819" s="11">
+    <row r="823" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A823" s="11">
         <v>50100887</v>
       </c>
-      <c r="B819" s="2" t="s">
+      <c r="B823" s="2" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="820" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A820" s="11">
+    <row r="824" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A824" s="11">
         <v>50109010</v>
       </c>
-      <c r="B820" s="2" t="s">
+      <c r="B824" s="2" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="821" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A821" s="11">
+    <row r="825" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A825" s="11">
         <v>50381970</v>
       </c>
-      <c r="B821" s="2" t="s">
+      <c r="B825" s="2" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="822" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A822" s="11">
+    <row r="826" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A826" s="11">
         <v>50077187</v>
       </c>
-      <c r="B822" s="2" t="s">
+      <c r="B826" s="2" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="823" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A823" s="11">
+    <row r="827" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A827" s="11">
         <v>50102832</v>
       </c>
-      <c r="B823" s="2" t="s">
+      <c r="B827" s="2" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="824" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A824" s="11">
+    <row r="828" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A828" s="11">
         <v>50109011</v>
       </c>
-      <c r="B824" s="2" t="s">
+      <c r="B828" s="2" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="825" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A825" s="11">
+    <row r="829" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A829" s="11">
         <v>50076093</v>
       </c>
-      <c r="B825" s="2" t="s">
+      <c r="B829" s="2" t="s">
         <v>174</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="0" firstPageNumber="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Adding fixed data for season 2016-2017, adding Pluimplukkers
</commit_message>
<xml_diff>
--- a/lf_front/data/fixed/2016-2017/Spelerslijst basisopstellingen.xlsx
+++ b/lf_front/data/fixed/2016-2017/Spelerslijst basisopstellingen.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17127"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -16,16 +16,11 @@
     <sheet name="ontbrekende" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="219">
   <si>
     <t>player_playerId</t>
   </si>
@@ -652,19 +647,56 @@
   </si>
   <si>
     <t>Wallabies 1G</t>
+  </si>
+  <si>
+    <t>50060437</t>
+  </si>
+  <si>
+    <t>50081259</t>
+  </si>
+  <si>
+    <t>50051489</t>
+  </si>
+  <si>
+    <t>50052910</t>
+  </si>
+  <si>
+    <t>50061387</t>
+  </si>
+  <si>
+    <t>50037837</t>
+  </si>
+  <si>
+    <t>50752057</t>
+  </si>
+  <si>
+    <t>50058438</t>
+  </si>
+  <si>
+    <t>50048606</t>
+  </si>
+  <si>
+    <t>50091428</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -696,6 +728,11 @@
       <sz val="10"/>
       <color rgb="FF505050"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -737,11 +774,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -751,34 +789,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard 2" xfId="2"/>
     <cellStyle name="Verklarende tekst" xfId="1" builtinId="53" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1161,8 +1214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK829"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A735" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B752" sqref="B752"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F568" sqref="F568"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6787,7 +6840,9 @@
       <c r="E553"/>
     </row>
     <row r="554" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A554" s="5"/>
+      <c r="A554" s="20" t="s">
+        <v>209</v>
+      </c>
       <c r="B554" s="3" t="s">
         <v>193</v>
       </c>
@@ -6795,7 +6850,9 @@
       <c r="E554"/>
     </row>
     <row r="555" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A555" s="5"/>
+      <c r="A555" s="20" t="s">
+        <v>210</v>
+      </c>
       <c r="B555" s="18" t="s">
         <v>193</v>
       </c>
@@ -6803,7 +6860,9 @@
       <c r="E555"/>
     </row>
     <row r="556" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A556" s="5"/>
+      <c r="A556" s="20" t="s">
+        <v>211</v>
+      </c>
       <c r="B556" s="18" t="s">
         <v>193</v>
       </c>
@@ -6811,7 +6870,9 @@
       <c r="E556"/>
     </row>
     <row r="557" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A557" s="5"/>
+      <c r="A557" s="20" t="s">
+        <v>212</v>
+      </c>
       <c r="B557" s="18" t="s">
         <v>193</v>
       </c>
@@ -6819,7 +6880,9 @@
       <c r="E557"/>
     </row>
     <row r="558" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A558" s="5"/>
+      <c r="A558" s="20" t="s">
+        <v>213</v>
+      </c>
       <c r="B558" s="3" t="s">
         <v>195</v>
       </c>
@@ -6827,7 +6890,9 @@
       <c r="E558"/>
     </row>
     <row r="559" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A559" s="5"/>
+      <c r="A559" s="20" t="s">
+        <v>214</v>
+      </c>
       <c r="B559" s="3" t="s">
         <v>195</v>
       </c>
@@ -6835,7 +6900,9 @@
       <c r="E559"/>
     </row>
     <row r="560" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A560" s="5"/>
+      <c r="A560" s="20" t="s">
+        <v>215</v>
+      </c>
       <c r="B560" s="3" t="s">
         <v>195</v>
       </c>
@@ -6843,328 +6910,410 @@
       <c r="E560"/>
     </row>
     <row r="561" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A561" s="5"/>
-      <c r="B561" s="3" t="s">
+      <c r="A561" s="21">
+        <v>50102294</v>
+      </c>
+      <c r="B561" s="22" t="s">
         <v>195</v>
       </c>
       <c r="D561"/>
       <c r="E561"/>
     </row>
     <row r="562" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A562" s="5"/>
-      <c r="B562" s="3" t="s">
+      <c r="A562" s="23">
+        <v>50093929</v>
+      </c>
+      <c r="B562" s="22" t="s">
         <v>197</v>
       </c>
       <c r="D562"/>
       <c r="E562"/>
     </row>
     <row r="563" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A563" s="5"/>
-      <c r="B563" s="3" t="s">
+      <c r="A563" s="23">
+        <v>50089191</v>
+      </c>
+      <c r="B563" s="22" t="s">
         <v>197</v>
       </c>
       <c r="D563"/>
       <c r="E563"/>
     </row>
     <row r="564" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A564" s="5"/>
-      <c r="B564" s="3" t="s">
+      <c r="A564" s="23">
+        <v>50085780</v>
+      </c>
+      <c r="B564" s="22" t="s">
         <v>197</v>
       </c>
       <c r="D564"/>
       <c r="E564"/>
     </row>
     <row r="565" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A565" s="5"/>
-      <c r="B565" s="3" t="s">
+      <c r="A565" s="23">
+        <v>50066435</v>
+      </c>
+      <c r="B565" s="22" t="s">
         <v>197</v>
       </c>
       <c r="D565"/>
       <c r="E565"/>
     </row>
     <row r="566" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A566" s="5"/>
-      <c r="B566" s="3" t="s">
+      <c r="A566" s="23">
+        <v>50012170</v>
+      </c>
+      <c r="B566" s="22" t="s">
         <v>199</v>
       </c>
       <c r="D566"/>
       <c r="E566"/>
     </row>
     <row r="567" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A567" s="5"/>
-      <c r="B567" s="3" t="s">
+      <c r="A567" s="23">
+        <v>50082279</v>
+      </c>
+      <c r="B567" s="22" t="s">
         <v>199</v>
       </c>
       <c r="D567"/>
       <c r="E567"/>
     </row>
     <row r="568" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A568" s="5"/>
-      <c r="B568" s="3" t="s">
+      <c r="A568" s="23">
+        <v>50080833</v>
+      </c>
+      <c r="B568" s="22" t="s">
         <v>199</v>
       </c>
       <c r="D568"/>
       <c r="E568"/>
     </row>
     <row r="569" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A569" s="5"/>
-      <c r="B569" s="3" t="s">
+      <c r="A569" s="23">
+        <v>50065725</v>
+      </c>
+      <c r="B569" s="22" t="s">
         <v>199</v>
       </c>
       <c r="D569"/>
       <c r="E569"/>
     </row>
     <row r="570" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A570" s="5"/>
-      <c r="B570" s="3" t="s">
+      <c r="A570" s="21">
+        <v>50056041</v>
+      </c>
+      <c r="B570" s="22" t="s">
         <v>190</v>
       </c>
       <c r="D570"/>
       <c r="E570"/>
     </row>
     <row r="571" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A571" s="5"/>
-      <c r="B571" s="3" t="s">
+      <c r="A571" s="21">
+        <v>50052422</v>
+      </c>
+      <c r="B571" s="22" t="s">
         <v>190</v>
       </c>
       <c r="D571"/>
       <c r="E571"/>
     </row>
     <row r="572" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A572" s="5"/>
-      <c r="B572" s="3" t="s">
+      <c r="A572" s="24">
+        <v>50116755</v>
+      </c>
+      <c r="B572" s="22" t="s">
         <v>190</v>
       </c>
       <c r="D572"/>
       <c r="E572"/>
     </row>
     <row r="573" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A573" s="5"/>
-      <c r="B573" s="3" t="s">
+      <c r="A573" s="24">
+        <v>50048706</v>
+      </c>
+      <c r="B573" s="22" t="s">
         <v>190</v>
       </c>
       <c r="D573"/>
       <c r="E573"/>
     </row>
     <row r="574" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A574" s="5"/>
-      <c r="B574" s="3" t="s">
+      <c r="A574" s="24">
+        <v>50011594</v>
+      </c>
+      <c r="B574" s="22" t="s">
         <v>191</v>
       </c>
       <c r="D574"/>
       <c r="E574"/>
     </row>
     <row r="575" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A575" s="5"/>
-      <c r="B575" s="3" t="s">
+      <c r="A575" s="24">
+        <v>50103067</v>
+      </c>
+      <c r="B575" s="22" t="s">
         <v>191</v>
       </c>
       <c r="D575"/>
       <c r="E575"/>
     </row>
     <row r="576" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A576" s="5"/>
-      <c r="B576" s="3" t="s">
+      <c r="A576" s="24">
+        <v>50073929</v>
+      </c>
+      <c r="B576" s="22" t="s">
         <v>191</v>
       </c>
       <c r="D576"/>
       <c r="E576"/>
     </row>
     <row r="577" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A577" s="5"/>
-      <c r="B577" s="3" t="s">
+      <c r="A577" s="24">
+        <v>50091505</v>
+      </c>
+      <c r="B577" s="22" t="s">
         <v>191</v>
       </c>
       <c r="D577"/>
       <c r="E577"/>
     </row>
     <row r="578" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A578" s="5"/>
-      <c r="B578" s="3" t="s">
+      <c r="A578" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="B578" s="22" t="s">
         <v>192</v>
       </c>
       <c r="D578"/>
       <c r="E578"/>
     </row>
     <row r="579" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A579" s="5"/>
-      <c r="B579" s="3" t="s">
+      <c r="A579" s="21" t="s">
+        <v>217</v>
+      </c>
+      <c r="B579" s="22" t="s">
         <v>192</v>
       </c>
       <c r="D579"/>
       <c r="E579"/>
     </row>
     <row r="580" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A580" s="5"/>
-      <c r="B580" s="3" t="s">
+      <c r="A580" s="21" t="s">
+        <v>218</v>
+      </c>
+      <c r="B580" s="22" t="s">
         <v>192</v>
       </c>
       <c r="D580"/>
       <c r="E580"/>
     </row>
     <row r="581" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A581" s="5"/>
-      <c r="B581" s="3" t="s">
+      <c r="A581" s="21">
+        <v>50052422</v>
+      </c>
+      <c r="B581" s="22" t="s">
         <v>192</v>
       </c>
       <c r="D581"/>
       <c r="E581"/>
     </row>
     <row r="582" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A582" s="5"/>
-      <c r="B582" s="3" t="s">
+      <c r="A582" s="25">
+        <v>50080643</v>
+      </c>
+      <c r="B582" s="22" t="s">
         <v>194</v>
       </c>
       <c r="D582"/>
       <c r="E582"/>
     </row>
     <row r="583" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A583" s="5"/>
-      <c r="B583" s="3" t="s">
+      <c r="A583" s="25">
+        <v>50061578</v>
+      </c>
+      <c r="B583" s="22" t="s">
         <v>194</v>
       </c>
       <c r="D583"/>
       <c r="E583"/>
     </row>
     <row r="584" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A584" s="5"/>
-      <c r="B584" s="3" t="s">
+      <c r="A584" s="25">
+        <v>50048706</v>
+      </c>
+      <c r="B584" s="22" t="s">
         <v>194</v>
       </c>
       <c r="D584"/>
       <c r="E584"/>
     </row>
     <row r="585" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A585" s="5"/>
-      <c r="B585" s="3" t="s">
+      <c r="A585" s="25">
+        <v>50104831</v>
+      </c>
+      <c r="B585" s="22" t="s">
         <v>194</v>
       </c>
       <c r="D585"/>
       <c r="E585"/>
     </row>
     <row r="586" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A586" s="5"/>
-      <c r="B586" s="3" t="s">
+      <c r="A586" s="25">
+        <v>50082610</v>
+      </c>
+      <c r="B586" s="22" t="s">
         <v>196</v>
       </c>
       <c r="D586"/>
       <c r="E586"/>
     </row>
     <row r="587" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A587" s="5"/>
-      <c r="B587" s="3" t="s">
+      <c r="A587" s="25">
+        <v>50060437</v>
+      </c>
+      <c r="B587" s="22" t="s">
         <v>196</v>
       </c>
       <c r="D587"/>
       <c r="E587"/>
     </row>
     <row r="588" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A588" s="5"/>
-      <c r="B588" s="3" t="s">
+      <c r="A588" s="25">
+        <v>50116755</v>
+      </c>
+      <c r="B588" s="22" t="s">
         <v>196</v>
       </c>
       <c r="D588"/>
       <c r="E588"/>
     </row>
     <row r="589" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A589" s="5"/>
-      <c r="B589" s="3" t="s">
+      <c r="A589" s="25">
+        <v>50103067</v>
+      </c>
+      <c r="B589" s="22" t="s">
         <v>196</v>
       </c>
       <c r="D589"/>
       <c r="E589"/>
     </row>
     <row r="590" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A590" s="5"/>
-      <c r="B590" s="3" t="s">
+      <c r="A590" s="25">
+        <v>50061387</v>
+      </c>
+      <c r="B590" s="22" t="s">
         <v>198</v>
       </c>
       <c r="D590"/>
       <c r="E590"/>
     </row>
     <row r="591" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A591" s="5"/>
-      <c r="B591" s="3" t="s">
+      <c r="A591" s="25">
+        <v>50081259</v>
+      </c>
+      <c r="B591" s="22" t="s">
         <v>198</v>
       </c>
       <c r="D591"/>
       <c r="E591"/>
     </row>
     <row r="592" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A592" s="5"/>
-      <c r="B592" s="3" t="s">
+      <c r="A592" s="25">
+        <v>50011594</v>
+      </c>
+      <c r="B592" s="22" t="s">
         <v>198</v>
       </c>
       <c r="D592"/>
       <c r="E592"/>
     </row>
     <row r="593" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A593" s="5"/>
-      <c r="B593" s="3" t="s">
+      <c r="A593" s="25">
+        <v>50066806</v>
+      </c>
+      <c r="B593" s="22" t="s">
         <v>198</v>
       </c>
       <c r="D593"/>
       <c r="E593"/>
     </row>
     <row r="594" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A594" s="5"/>
-      <c r="B594" s="3" t="s">
+      <c r="A594" s="25">
+        <v>50102294</v>
+      </c>
+      <c r="B594" s="22" t="s">
         <v>200</v>
       </c>
       <c r="D594"/>
       <c r="E594"/>
     </row>
     <row r="595" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A595" s="5"/>
-      <c r="B595" s="3" t="s">
+      <c r="A595" s="25">
+        <v>50051489</v>
+      </c>
+      <c r="B595" s="22" t="s">
         <v>200</v>
       </c>
       <c r="D595"/>
       <c r="E595"/>
     </row>
     <row r="596" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A596" s="5"/>
-      <c r="B596" s="3" t="s">
+      <c r="A596" s="25">
+        <v>50073929</v>
+      </c>
+      <c r="B596" s="22" t="s">
         <v>200</v>
       </c>
       <c r="D596"/>
       <c r="E596"/>
     </row>
     <row r="597" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A597" s="5"/>
-      <c r="B597" s="3" t="s">
+      <c r="A597" s="25">
+        <v>50091505</v>
+      </c>
+      <c r="B597" s="22" t="s">
         <v>200</v>
       </c>
       <c r="D597"/>
       <c r="E597"/>
     </row>
     <row r="598" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A598" s="5"/>
-      <c r="B598" s="3" t="s">
+      <c r="A598" s="25">
+        <v>50037837</v>
+      </c>
+      <c r="B598" s="22" t="s">
         <v>201</v>
       </c>
       <c r="D598"/>
       <c r="E598"/>
     </row>
     <row r="599" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A599" s="5"/>
-      <c r="B599" s="3" t="s">
+      <c r="A599" s="25">
+        <v>50052910</v>
+      </c>
+      <c r="B599" s="22" t="s">
         <v>201</v>
       </c>
       <c r="D599"/>
       <c r="E599"/>
     </row>
     <row r="600" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A600" s="5"/>
-      <c r="B600" s="3" t="s">
+      <c r="A600" s="25">
+        <v>50105176</v>
+      </c>
+      <c r="B600" s="22" t="s">
         <v>201</v>
       </c>
       <c r="D600"/>
       <c r="E600"/>
     </row>
     <row r="601" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A601" s="5"/>
-      <c r="B601" s="3" t="s">
+      <c r="A601" s="25">
+        <v>50109412</v>
+      </c>
+      <c r="B601" s="22" t="s">
         <v>201</v>
       </c>
       <c r="D601"/>
@@ -9439,7 +9588,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:A26"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>